<commit_message>
Generated IG's after updating fhirpath in condition profile and fixing bus in patient ihi profile.
</commit_message>
<xml_diff>
--- a/output/EventSummary/condition-summary-1.xlsx
+++ b/output/EventSummary/condition-summary-1.xlsx
@@ -156,7 +156,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}con-4:If condition is abated, then clinicalStatus must be either inactive, resolved, or remission {abatement.empty() or (abatement as boolean).not()  or clinicalStatus='resolved' or clinicalStatus='remission' or clinicalStatus='inactive'}con-3:Condition.clinicalStatus SHALL be present if verificationStatus is not entered-in-error {verificationStatus='entered-in-error' or clinicalStatus.exists()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}con-4:If condition is abated, then clinicalStatus must be either inactive, resolved, or remission {abatement.empty() or (abatement as boolean).not()  or clinicalStatus='resolved' or clinicalStatus='remission' or clinicalStatus='inactive'}con-3:Condition.clinicalStatus SHALL be present if verificationStatus is not entered-in-error {verificationStatus='entered-in-error' or clinicalStatus.exists()}inv-dh-cond-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-cond-03:If present, a recorder shall at least have a reference, an identifier or a display {recorder.exists() implies recorder.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}</t>
   </si>
   <si>
     <t>&lt; 243796009 |Situation with explicit context|:
@@ -356,10 +356,10 @@
 </t>
   </si>
   <si>
-    <t>Who recorded the condition</t>
-  </si>
-  <si>
-    <t>Reference to an individual who recorded the condition and takes responsibility for its content.</t>
+    <t>Who recorded the record</t>
+  </si>
+  <si>
+    <t>Individual who recorded the record and takes responsibility for its content.</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -367,7 +367,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cond-02:A practitioner shall conform to Base Practitioner, a patient shall conform to Base Patient, and a related person shall conform to Base RelatedPerson {Condition.extension('http://hl7.org.au/fhir/StructureDefinition/recorder').where(resolve() is Practitioner implies resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-dh-base-1')) and Condition.extension('http://hl7.org.au/fhir/StructureDefinition/recorder').where(resolve() is Patient implies resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-dh-base-1')) and Condition.extension('http://hl7.org.au/fhir/StructureDefinition/recorder').where(resolve() is RelatedPerson implies resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1'))}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cond-02:A practitioner shall conform to Base Practitioner, a patient shall conform to Base Patient, and a related person shall conform to Base RelatedPerson {all($this.valueReference.reference.exists() implies ($this.valueReference.reference.resolve().where($this is Practitioner).conformsTo('http://hl7.org/fhir/StructureDefinition/Practitioner') or $this.valueReference.reference.resolve().where($this is Patient).conformsTo('http://hl7.org/fhir/StructureDefinition/Patient') or $this.valueReference.reference.resolve().where($this is RelatedPerson).conformsTo('http://hl7.org/fhir/StructureDefinition/RelatedPerson')))}</t>
   </si>
   <si>
     <t>Condition.modifierExtension</t>

</xml_diff>